<commit_message>
Added tests for to_excel() parameters with xlsxwriter.
</commit_message>
<xml_diff>
--- a/pandas/io/tests/data/xw_frame01.xlsx
+++ b/pandas/io/tests/data/xw_frame01.xlsx
@@ -11,23 +11,6 @@
   </sheets>
   <calcPr calcId="124519"/>
 </workbook>
-</file>
-
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
-  <si>
-    <t>foo</t>
-  </si>
-  <si>
-    <t>bar</t>
-  </si>
-  <si>
-    <t>bin</t>
-  </si>
-  <si>
-    <t>boo</t>
-  </si>
-</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -367,32 +350,32 @@
       <c r="A1">
         <v>10</v>
       </c>
-      <c r="B1" t="s">
-        <v>0</v>
+      <c r="B1">
+        <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:2">
       <c r="A2">
         <v>11</v>
       </c>
-      <c r="B2" t="s">
-        <v>1</v>
+      <c r="B2">
+        <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3">
         <v>12</v>
       </c>
-      <c r="B3" t="s">
-        <v>2</v>
+      <c r="B3">
+        <v>6</v>
       </c>
     </row>
     <row r="4" spans="1:2">
       <c r="A4">
         <v>13</v>
       </c>
-      <c r="B4" t="s">
-        <v>3</v>
+      <c r="B4">
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>